<commit_message>
zh-tW -> Eng to test embedding,and refind qa_type
</commit_message>
<xml_diff>
--- a/test_questions.xlsx
+++ b/test_questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zirong/Desktop/CCD_RAG/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5641E6C-D5F5-8149-8EA7-1F468B156A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49FFCD62-EBC6-7D4E-987E-FC4C18007F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4060" yWindow="740" windowWidth="19680" windowHeight="17100" xr2:uid="{49CF8178-EFA8-9643-BFB1-A8E39845DF37}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="129">
   <si>
     <t>我的臘腸狗已經 13 歲，最近總是在半夜突然狂吠，轉圈找不到床，還弄得全家都睡不著。白天牠又一直昏睡、反應遲鈍。我懷疑可能是 CCD，但不確定要怎麼做？請問如何判斷是不是失智，還有夜間吠叫該怎麼安撫或調整作息？</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -146,17 +146,6 @@
   </si>
   <si>
     <t>大中小型狗的失智照顧方式有什麼不同？</t>
-  </si>
-  <si>
-    <t>問答</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>是非</t>
-  </si>
-  <si>
-    <t>是非</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>發炎反應 (pro-inflammatory cytokines) 升高，可能加速神經退化。神經遞質 (serotonin, GABA) 與免疫調控 (短鏈脂肪酸, SCFAs) 的影響。腸道微生物與中樞神經系統之間的交互作用。</t>
@@ -242,9 +231,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>選擇</t>
-  </si>
-  <si>
     <t>照護</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -653,6 +639,27 @@
   </si>
   <si>
     <t>針對犬隻失智 (CCD) 的診斷，是否可以單靠 MRI 或 CT 等影像學觀察大腦萎縮或斑塊沉積，即可準確區分 CCD 與其他神經退化疾病。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>true_false</t>
+  </si>
+  <si>
+    <t>multiple_choice</t>
+  </si>
+  <si>
+    <t>multiple_choice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true_false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qa</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1123,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27A6E25-28F7-6A43-9063-8BB9C579CCE6}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -1139,19 +1146,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="10" customFormat="1">
       <c r="A1" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>45</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>5</v>
@@ -1162,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -1182,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>1</v>
@@ -1202,16 +1209,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>7</v>
@@ -1222,16 +1229,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>7</v>
@@ -1242,16 +1249,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>7</v>
@@ -1262,7 +1269,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>4</v>
@@ -1271,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>8</v>
@@ -1282,7 +1289,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
@@ -1291,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>8</v>
@@ -1302,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>9</v>
@@ -1311,7 +1318,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>8</v>
@@ -1322,7 +1329,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>11</v>
@@ -1342,7 +1349,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>14</v>
@@ -1354,7 +1361,7 @@
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="32">
@@ -1362,7 +1369,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>16</v>
@@ -1382,7 +1389,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>18</v>
@@ -1391,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F13" s="5" t="s">
         <v>8</v>
@@ -1402,16 +1409,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D14" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>8</v>
@@ -1422,7 +1429,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>19</v>
@@ -1431,7 +1438,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>8</v>
@@ -1442,7 +1449,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>20</v>
@@ -1454,7 +1461,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="32">
@@ -1462,7 +1469,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>22</v>
@@ -1471,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>8</v>
@@ -1482,7 +1489,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>23</v>
@@ -1500,19 +1507,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="320">
@@ -1520,19 +1527,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>28</v>
+        <v>128</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="144">
@@ -1540,19 +1547,19 @@
         <v>21</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="7" t="s">
         <v>34</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="272">
@@ -1560,19 +1567,19 @@
         <v>22</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="272">
@@ -1580,19 +1587,19 @@
         <v>23</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="96">
@@ -1600,19 +1607,19 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="F24" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="96">
@@ -1620,19 +1627,19 @@
         <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="96">
@@ -1640,19 +1647,19 @@
         <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="96">
@@ -1660,19 +1667,19 @@
         <v>27</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="96">
@@ -1680,19 +1687,19 @@
         <v>28</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="112">
@@ -1700,19 +1707,19 @@
         <v>29</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="96">
@@ -1720,19 +1727,19 @@
         <v>30</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="96">
@@ -1740,19 +1747,19 @@
         <v>31</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="96">
@@ -1760,19 +1767,19 @@
         <v>32</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="96">
@@ -1780,19 +1787,19 @@
         <v>33</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="96">
@@ -1800,19 +1807,19 @@
         <v>34</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="96">
@@ -1820,19 +1827,19 @@
         <v>35</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="96">
@@ -1840,19 +1847,19 @@
         <v>36</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="96">
@@ -1860,19 +1867,19 @@
         <v>37</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="96">
@@ -1880,19 +1887,19 @@
         <v>38</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="48">
@@ -1900,19 +1907,19 @@
         <v>39</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D39" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="32">
@@ -1920,19 +1927,19 @@
         <v>40</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D40" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="48">
@@ -1940,19 +1947,19 @@
         <v>41</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D41" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="48">
@@ -1960,19 +1967,19 @@
         <v>42</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D42" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="32">
@@ -1980,19 +1987,19 @@
         <v>43</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D43" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="48">
@@ -2000,19 +2007,19 @@
         <v>44</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D44" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="32">
@@ -2020,19 +2027,19 @@
         <v>45</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D45" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="32">
@@ -2040,19 +2047,19 @@
         <v>46</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D46" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="32">
@@ -2060,19 +2067,19 @@
         <v>47</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D47" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="32">
@@ -2080,19 +2087,19 @@
         <v>48</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D48" s="11" t="b">
         <v>0</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="32">
@@ -2100,19 +2107,19 @@
         <v>49</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D49" s="11" t="b">
         <v>1</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="48">
@@ -2120,19 +2127,19 @@
         <v>50</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="140">
@@ -2140,16 +2147,16 @@
         <v>51</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>8</v>
@@ -2160,16 +2167,16 @@
         <v>52</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>46</v>
+        <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>8</v>
@@ -2180,16 +2187,16 @@
         <v>53</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E53" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>8</v>
@@ -2200,16 +2207,16 @@
         <v>54</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>8</v>
@@ -2220,16 +2227,16 @@
         <v>55</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>30</v>
+        <v>127</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D55" s="15" t="b">
         <v>0</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>8</v>
@@ -2240,16 +2247,16 @@
         <v>56</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>30</v>
+        <v>124</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D56" s="15" t="b">
         <v>0</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>8</v>

</xml_diff>